<commit_message>
punto 2 tp2 WIP
</commit_message>
<xml_diff>
--- a/tp2/docs/progdinamica_pto2.xlsx
+++ b/tp2/docs/progdinamica_pto2.xlsx
@@ -99,7 +99,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Comprar todo lo que se pueda en el mes 1(20), todo lo que se pueda en el mes 2(11), lo que sobre en el 3(0)
+Comprar todo lo que se pueda en el mes 1(20), lo del mes 2(2), lo que sobre en el 3(9)
 </t>
         </r>
       </text>
@@ -149,7 +149,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Comprar todo lo que se pueda en el mes 1 (20), lo optimo del mes 2 (12), lo que sobre en el mes 3(1)</t>
+Comprar lo optimo del mes 1 (10), todo lo que se pueda en el mes 2 (20), lo que sobre en el mes 3(1)</t>
         </r>
       </text>
     </comment>
@@ -212,29 +212,40 @@
     <t>Min</t>
   </si>
   <si>
-    <t>Q:10, Costo=2</t>
-  </si>
-  <si>
     <t>Q:2, Costo=2+4*10+2=44</t>
   </si>
   <si>
-    <t>Q: 1, Costo=4+8*1+2=14</t>
-  </si>
-  <si>
-    <t>Q:9, Costo=4+2=6</t>
-  </si>
-  <si>
-    <t>Q: 0, Costo=44+9*10=136</t>
-  </si>
-  <si>
-    <t>Q:12, Costo=2+2=4*</t>
+    <r>
+      <t>Q:12, Costo=2+2=4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>▪</t>
+    </r>
+  </si>
+  <si>
+    <t>Q:10, Costo=2▪</t>
+  </si>
+  <si>
+    <t>Q:9, Costo=4+2=6▪</t>
+  </si>
+  <si>
+    <t>Q:1, Costo=2+2+8*4+2=38</t>
+  </si>
+  <si>
+    <t>Q: 9, Costo= 2+4*10+2+2=46</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +278,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -674,7 +691,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +699,7 @@
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -760,24 +777,24 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
       <c r="D10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,6 +836,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>